<commit_message>
Code gen getting closer.
</commit_message>
<xml_diff>
--- a/KC-390_DBD_Enums.xlsx
+++ b/KC-390_DBD_Enums.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="382">
   <si>
     <t>ENUM-Message_ID</t>
   </si>
@@ -557,9 +557,6 @@
     <t>Compatibility Fault</t>
   </si>
   <si>
-    <t>None/OFF</t>
-  </si>
-  <si>
     <t>RED</t>
   </si>
   <si>
@@ -677,15 +674,6 @@
     <t>OK (Button 1 - Button 2 is not visible)</t>
   </si>
   <si>
-    <t>normal</t>
-  </si>
-  <si>
-    <t>yellow (not used)</t>
-  </si>
-  <si>
-    <t>red</t>
-  </si>
-  <si>
     <t>READY</t>
   </si>
   <si>
@@ -1158,6 +1146,21 @@
   </si>
   <si>
     <t>Pos_445</t>
+  </si>
+  <si>
+    <t>Bkg_Normal</t>
+  </si>
+  <si>
+    <t>Bkg_Yellow</t>
+  </si>
+  <si>
+    <t>Bkg_Red</t>
+  </si>
+  <si>
+    <t>No_Lock</t>
+  </si>
+  <si>
+    <t>No PDM</t>
   </si>
 </sst>
 </file>
@@ -1513,8 +1516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F412"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A348" workbookViewId="0">
-      <selection activeCell="B368" sqref="B368"/>
+    <sheetView tabSelected="1" topLeftCell="A387" workbookViewId="0">
+      <selection activeCell="B413" sqref="B413"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1527,13 +1530,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="B1" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="C1" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -2816,7 +2819,7 @@
         <v>0</v>
       </c>
       <c r="B150" t="s">
-        <v>180</v>
+        <v>292</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
@@ -2824,7 +2827,7 @@
         <v>1</v>
       </c>
       <c r="B151" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
@@ -2832,7 +2835,7 @@
         <v>2</v>
       </c>
       <c r="B152" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
@@ -2840,12 +2843,12 @@
         <v>3</v>
       </c>
       <c r="B153" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
@@ -2853,7 +2856,7 @@
         <v>0</v>
       </c>
       <c r="B155" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
@@ -2861,7 +2864,7 @@
         <v>1</v>
       </c>
       <c r="B156" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
@@ -2869,7 +2872,7 @@
         <v>2</v>
       </c>
       <c r="B157" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
@@ -2882,7 +2885,7 @@
         <v>0</v>
       </c>
       <c r="B159" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
@@ -2890,7 +2893,7 @@
         <v>1</v>
       </c>
       <c r="B160" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.3">
@@ -2898,7 +2901,7 @@
         <v>2</v>
       </c>
       <c r="B161" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.3">
@@ -2906,7 +2909,7 @@
         <v>3</v>
       </c>
       <c r="B162" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.3">
@@ -2914,7 +2917,7 @@
         <v>4</v>
       </c>
       <c r="B163" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.3">
@@ -2922,7 +2925,7 @@
         <v>5</v>
       </c>
       <c r="B164" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.3">
@@ -2930,7 +2933,7 @@
         <v>6</v>
       </c>
       <c r="B165" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.3">
@@ -2938,7 +2941,7 @@
         <v>7</v>
       </c>
       <c r="B166" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.3">
@@ -2946,7 +2949,7 @@
         <v>8</v>
       </c>
       <c r="B167" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.3">
@@ -2954,7 +2957,7 @@
         <v>9</v>
       </c>
       <c r="B168" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.3">
@@ -2962,7 +2965,7 @@
         <v>10</v>
       </c>
       <c r="B169" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.3">
@@ -2970,7 +2973,7 @@
         <v>11</v>
       </c>
       <c r="B170" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.3">
@@ -2978,7 +2981,7 @@
         <v>12</v>
       </c>
       <c r="B171" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.3">
@@ -2986,7 +2989,7 @@
         <v>13</v>
       </c>
       <c r="B172" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.3">
@@ -2994,7 +2997,7 @@
         <v>14</v>
       </c>
       <c r="B173" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.3">
@@ -3002,7 +3005,7 @@
         <v>15</v>
       </c>
       <c r="B174" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.3">
@@ -3010,7 +3013,7 @@
         <v>16</v>
       </c>
       <c r="B175" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.3">
@@ -3026,7 +3029,7 @@
         <v>18</v>
       </c>
       <c r="B177" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.3">
@@ -3034,7 +3037,7 @@
         <v>19</v>
       </c>
       <c r="B178" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.3">
@@ -3042,7 +3045,7 @@
         <v>20</v>
       </c>
       <c r="B179" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.3">
@@ -3050,7 +3053,7 @@
         <v>21</v>
       </c>
       <c r="B180" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.3">
@@ -3058,12 +3061,12 @@
         <v>22</v>
       </c>
       <c r="B181" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.3">
@@ -3071,7 +3074,7 @@
         <v>1</v>
       </c>
       <c r="B183" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.3">
@@ -3079,7 +3082,7 @@
         <v>2</v>
       </c>
       <c r="B184" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.3">
@@ -3087,7 +3090,7 @@
         <v>3</v>
       </c>
       <c r="B185" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.3">
@@ -3100,7 +3103,7 @@
         <v>0</v>
       </c>
       <c r="B187" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.3">
@@ -3108,7 +3111,7 @@
         <v>1</v>
       </c>
       <c r="B188" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.3">
@@ -3116,7 +3119,7 @@
         <v>2</v>
       </c>
       <c r="B189" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.3">
@@ -3129,7 +3132,7 @@
         <v>0</v>
       </c>
       <c r="B191" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.3">
@@ -3137,7 +3140,7 @@
         <v>1</v>
       </c>
       <c r="B192" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.3">
@@ -3145,7 +3148,7 @@
         <v>2</v>
       </c>
       <c r="B193" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.3">
@@ -3158,7 +3161,7 @@
         <v>0</v>
       </c>
       <c r="B195" t="s">
-        <v>220</v>
+        <v>377</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.3">
@@ -3166,7 +3169,7 @@
         <v>1</v>
       </c>
       <c r="B196" t="s">
-        <v>221</v>
+        <v>378</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.3">
@@ -3174,7 +3177,7 @@
         <v>2</v>
       </c>
       <c r="B197" t="s">
-        <v>222</v>
+        <v>379</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.3">
@@ -3187,7 +3190,7 @@
         <v>1</v>
       </c>
       <c r="B199" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.3">
@@ -3195,7 +3198,7 @@
         <v>2</v>
       </c>
       <c r="B200" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.3">
@@ -3203,7 +3206,7 @@
         <v>3</v>
       </c>
       <c r="B201" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.3">
@@ -3211,7 +3214,7 @@
         <v>4</v>
       </c>
       <c r="B202" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.3">
@@ -3219,7 +3222,7 @@
         <v>5</v>
       </c>
       <c r="B203" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.3">
@@ -3232,7 +3235,7 @@
         <v>0</v>
       </c>
       <c r="B205" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.3">
@@ -3240,7 +3243,7 @@
         <v>1</v>
       </c>
       <c r="B206" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.3">
@@ -3253,7 +3256,7 @@
         <v>0</v>
       </c>
       <c r="B208" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.3">
@@ -3261,7 +3264,7 @@
         <v>1</v>
       </c>
       <c r="B209" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.3">
@@ -3269,7 +3272,7 @@
         <v>2</v>
       </c>
       <c r="B210" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.3">
@@ -3277,7 +3280,7 @@
         <v>3</v>
       </c>
       <c r="B211" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.3">
@@ -3285,7 +3288,7 @@
         <v>4</v>
       </c>
       <c r="B212" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.3">
@@ -3293,7 +3296,7 @@
         <v>5</v>
       </c>
       <c r="B213" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.3">
@@ -3301,12 +3304,12 @@
         <v>6</v>
       </c>
       <c r="B214" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.3">
@@ -3314,7 +3317,7 @@
         <v>0</v>
       </c>
       <c r="B216" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.3">
@@ -3322,12 +3325,12 @@
         <v>1</v>
       </c>
       <c r="B217" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.3">
@@ -3335,7 +3338,7 @@
         <v>0</v>
       </c>
       <c r="B219" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.3">
@@ -3343,7 +3346,7 @@
         <v>1</v>
       </c>
       <c r="B220" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.3">
@@ -3351,7 +3354,7 @@
         <v>2</v>
       </c>
       <c r="B221" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.3">
@@ -3364,7 +3367,7 @@
         <v>0</v>
       </c>
       <c r="B223" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.3">
@@ -3372,7 +3375,7 @@
         <v>1</v>
       </c>
       <c r="B224" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.3">
@@ -3380,7 +3383,7 @@
         <v>2</v>
       </c>
       <c r="B225" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.3">
@@ -3388,15 +3391,15 @@
         <v>3</v>
       </c>
       <c r="B226" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227" s="1" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="D227" s="1" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.3">
@@ -3404,7 +3407,7 @@
         <v>0</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.3">
@@ -3412,7 +3415,7 @@
         <v>1</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.3">
@@ -3420,7 +3423,7 @@
         <v>2</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.3">
@@ -3433,7 +3436,7 @@
         <v>0</v>
       </c>
       <c r="B232" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.3">
@@ -3441,7 +3444,7 @@
         <v>1</v>
       </c>
       <c r="B233" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.3">
@@ -3449,7 +3452,7 @@
         <v>2</v>
       </c>
       <c r="B234" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.3">
@@ -3457,7 +3460,7 @@
         <v>3</v>
       </c>
       <c r="B235" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.3">
@@ -3465,7 +3468,7 @@
         <v>4</v>
       </c>
       <c r="B236" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.3">
@@ -3478,7 +3481,7 @@
         <v>0</v>
       </c>
       <c r="B238" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.3">
@@ -3486,7 +3489,7 @@
         <v>1</v>
       </c>
       <c r="B239" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.3">
@@ -3494,7 +3497,7 @@
         <v>2</v>
       </c>
       <c r="B240" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.3">
@@ -3502,7 +3505,7 @@
         <v>3</v>
       </c>
       <c r="B241" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.3">
@@ -3515,7 +3518,7 @@
         <v>0</v>
       </c>
       <c r="B243" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.3">
@@ -3523,7 +3526,7 @@
         <v>1</v>
       </c>
       <c r="B244" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.3">
@@ -3531,7 +3534,7 @@
         <v>2</v>
       </c>
       <c r="B245" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.3">
@@ -3539,7 +3542,7 @@
         <v>3</v>
       </c>
       <c r="B246" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.3">
@@ -3547,7 +3550,7 @@
         <v>4</v>
       </c>
       <c r="B247" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.3">
@@ -3560,7 +3563,7 @@
         <v>0</v>
       </c>
       <c r="B249" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.3">
@@ -3568,7 +3571,7 @@
         <v>1</v>
       </c>
       <c r="B250" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.3">
@@ -3576,7 +3579,7 @@
         <v>2</v>
       </c>
       <c r="B251" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.3">
@@ -3584,7 +3587,7 @@
         <v>3</v>
       </c>
       <c r="B252" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.3">
@@ -3592,7 +3595,7 @@
         <v>4</v>
       </c>
       <c r="B253" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.3">
@@ -3605,7 +3608,7 @@
         <v>0</v>
       </c>
       <c r="B255" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.3">
@@ -3613,7 +3616,7 @@
         <v>1</v>
       </c>
       <c r="B256" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.3">
@@ -3626,7 +3629,7 @@
         <v>0</v>
       </c>
       <c r="B258" t="s">
-        <v>266</v>
+        <v>380</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.3">
@@ -3634,7 +3637,7 @@
         <v>1</v>
       </c>
       <c r="B259" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.3">
@@ -3642,7 +3645,7 @@
         <v>2</v>
       </c>
       <c r="B260" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.3">
@@ -3650,7 +3653,7 @@
         <v>3</v>
       </c>
       <c r="B261" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.3">
@@ -3658,7 +3661,7 @@
         <v>4</v>
       </c>
       <c r="B262" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.3">
@@ -3666,7 +3669,7 @@
         <v>5</v>
       </c>
       <c r="B263" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.3">
@@ -3674,7 +3677,7 @@
         <v>6</v>
       </c>
       <c r="B264" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.3">
@@ -3682,7 +3685,7 @@
         <v>7</v>
       </c>
       <c r="B265" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.3">
@@ -3690,7 +3693,7 @@
         <v>8</v>
       </c>
       <c r="B266" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.3">
@@ -3698,7 +3701,7 @@
         <v>9</v>
       </c>
       <c r="B267" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.3">
@@ -3706,7 +3709,7 @@
         <v>10</v>
       </c>
       <c r="B268" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.3">
@@ -3714,7 +3717,7 @@
         <v>11</v>
       </c>
       <c r="B269" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.3">
@@ -3722,7 +3725,7 @@
         <v>12</v>
       </c>
       <c r="B270" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.3">
@@ -3730,7 +3733,7 @@
         <v>13</v>
       </c>
       <c r="B271" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.3">
@@ -3738,7 +3741,7 @@
         <v>14</v>
       </c>
       <c r="B272" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.3">
@@ -3746,7 +3749,7 @@
         <v>15</v>
       </c>
       <c r="B273" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.3">
@@ -3754,7 +3757,7 @@
         <v>16</v>
       </c>
       <c r="B274" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.3">
@@ -3767,7 +3770,7 @@
         <v>0</v>
       </c>
       <c r="B276" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.3">
@@ -3783,7 +3786,7 @@
         <v>2</v>
       </c>
       <c r="B278" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.3">
@@ -3791,7 +3794,7 @@
         <v>3</v>
       </c>
       <c r="B279" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.3">
@@ -3799,7 +3802,7 @@
         <v>4</v>
       </c>
       <c r="B280" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.3">
@@ -3807,7 +3810,7 @@
         <v>5</v>
       </c>
       <c r="B281" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.3">
@@ -3815,7 +3818,7 @@
         <v>6</v>
       </c>
       <c r="B282" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.3">
@@ -3823,7 +3826,7 @@
         <v>7</v>
       </c>
       <c r="B283" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.3">
@@ -3831,7 +3834,7 @@
         <v>8</v>
       </c>
       <c r="B284" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.3">
@@ -3839,7 +3842,7 @@
         <v>9</v>
       </c>
       <c r="B285" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.3">
@@ -3847,7 +3850,7 @@
         <v>10</v>
       </c>
       <c r="B286" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.3">
@@ -3860,7 +3863,7 @@
         <v>0</v>
       </c>
       <c r="B288" t="s">
-        <v>266</v>
+        <v>381</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.3">
@@ -3868,7 +3871,7 @@
         <v>1</v>
       </c>
       <c r="B289" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.3">
@@ -3876,7 +3879,7 @@
         <v>2</v>
       </c>
       <c r="B290" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.3">
@@ -3889,7 +3892,7 @@
         <v>0</v>
       </c>
       <c r="B292" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.3">
@@ -3897,7 +3900,7 @@
         <v>1</v>
       </c>
       <c r="B293" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.3">
@@ -3910,7 +3913,7 @@
         <v>0</v>
       </c>
       <c r="B295" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.3">
@@ -3918,7 +3921,7 @@
         <v>1</v>
       </c>
       <c r="B296" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.3">
@@ -3926,7 +3929,7 @@
         <v>2</v>
       </c>
       <c r="B297" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.3">
@@ -3934,7 +3937,7 @@
         <v>3</v>
       </c>
       <c r="B298" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.3">
@@ -3947,7 +3950,7 @@
         <v>0</v>
       </c>
       <c r="B300" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.3">
@@ -3955,7 +3958,7 @@
         <v>1</v>
       </c>
       <c r="B301" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.3">
@@ -3963,7 +3966,7 @@
         <v>2</v>
       </c>
       <c r="B302" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.3">
@@ -3971,12 +3974,12 @@
         <v>3</v>
       </c>
       <c r="B303" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.3">
@@ -3984,7 +3987,7 @@
         <v>0</v>
       </c>
       <c r="B305" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.3">
@@ -3992,7 +3995,7 @@
         <v>1</v>
       </c>
       <c r="B306" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.3">
@@ -4000,7 +4003,7 @@
         <v>2</v>
       </c>
       <c r="B307" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.3">
@@ -4008,12 +4011,12 @@
         <v>3</v>
       </c>
       <c r="B308" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.3">
@@ -4021,7 +4024,7 @@
         <v>0</v>
       </c>
       <c r="B310" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.3">
@@ -4029,7 +4032,7 @@
         <v>1</v>
       </c>
       <c r="B311" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.3">
@@ -4037,7 +4040,7 @@
         <v>2</v>
       </c>
       <c r="B312" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.3">
@@ -4045,7 +4048,7 @@
         <v>3</v>
       </c>
       <c r="B313" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.3">
@@ -4058,7 +4061,7 @@
         <v>0</v>
       </c>
       <c r="B315" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.3">
@@ -4066,12 +4069,12 @@
         <v>1</v>
       </c>
       <c r="B316" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.3">
@@ -4079,7 +4082,7 @@
         <v>0</v>
       </c>
       <c r="B318" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.3">
@@ -4087,7 +4090,7 @@
         <v>1</v>
       </c>
       <c r="B319" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.3">
@@ -4100,7 +4103,7 @@
         <v>0</v>
       </c>
       <c r="B321" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.3">
@@ -4108,7 +4111,7 @@
         <v>1</v>
       </c>
       <c r="B322" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.3">
@@ -4116,7 +4119,7 @@
         <v>2</v>
       </c>
       <c r="B323" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.3">
@@ -4124,7 +4127,7 @@
         <v>3</v>
       </c>
       <c r="B324" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.3">
@@ -4132,7 +4135,7 @@
         <v>4</v>
       </c>
       <c r="B325" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.3">
@@ -4140,7 +4143,7 @@
         <v>5</v>
       </c>
       <c r="B326" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.3">
@@ -4153,7 +4156,7 @@
         <v>1</v>
       </c>
       <c r="B328" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.3">
@@ -4161,7 +4164,7 @@
         <v>2</v>
       </c>
       <c r="B329" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.3">
@@ -4169,7 +4172,7 @@
         <v>3</v>
       </c>
       <c r="B330" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.3">
@@ -4177,7 +4180,7 @@
         <v>4</v>
       </c>
       <c r="B331" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.3">
@@ -4190,7 +4193,7 @@
         <v>0</v>
       </c>
       <c r="B333" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.3">
@@ -4198,7 +4201,7 @@
         <v>1</v>
       </c>
       <c r="B334" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.3">
@@ -4206,7 +4209,7 @@
         <v>2</v>
       </c>
       <c r="B335" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.3">
@@ -4214,7 +4217,7 @@
         <v>3</v>
       </c>
       <c r="B336" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.3">
@@ -4227,7 +4230,7 @@
         <v>1</v>
       </c>
       <c r="B338" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.3">
@@ -4235,7 +4238,7 @@
         <v>2</v>
       </c>
       <c r="B339" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.3">
@@ -4243,7 +4246,7 @@
         <v>3</v>
       </c>
       <c r="B340" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.3">
@@ -4251,7 +4254,7 @@
         <v>4</v>
       </c>
       <c r="B341" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.3">
@@ -4259,7 +4262,7 @@
         <v>5</v>
       </c>
       <c r="B342" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.3">
@@ -4267,7 +4270,7 @@
         <v>6</v>
       </c>
       <c r="B343" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.3">
@@ -4275,7 +4278,7 @@
         <v>7</v>
       </c>
       <c r="B344" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.3">
@@ -4283,7 +4286,7 @@
         <v>8</v>
       </c>
       <c r="B345" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.3">
@@ -4291,7 +4294,7 @@
         <v>9</v>
       </c>
       <c r="B346" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.3">
@@ -4299,7 +4302,7 @@
         <v>10</v>
       </c>
       <c r="B347" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.3">
@@ -4312,7 +4315,7 @@
         <v>0</v>
       </c>
       <c r="B349" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.3">
@@ -4320,7 +4323,7 @@
         <v>1</v>
       </c>
       <c r="B350" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.3">
@@ -4328,7 +4331,7 @@
         <v>2</v>
       </c>
       <c r="B351" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.3">
@@ -4336,12 +4339,12 @@
         <v>3</v>
       </c>
       <c r="B352" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.3">
@@ -4349,7 +4352,7 @@
         <v>0</v>
       </c>
       <c r="B354" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.3">
@@ -4357,7 +4360,7 @@
         <v>1</v>
       </c>
       <c r="B355" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.3">
@@ -4365,7 +4368,7 @@
         <v>2</v>
       </c>
       <c r="B356" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.3">
@@ -4373,7 +4376,7 @@
         <v>3</v>
       </c>
       <c r="B357" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.3">
@@ -4381,7 +4384,7 @@
         <v>4</v>
       </c>
       <c r="B358" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.3">
@@ -4389,7 +4392,7 @@
         <v>5</v>
       </c>
       <c r="B359" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.3">
@@ -4397,7 +4400,7 @@
         <v>6</v>
       </c>
       <c r="B360" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.3">
@@ -4405,7 +4408,7 @@
         <v>7</v>
       </c>
       <c r="B361" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.3">
@@ -4413,7 +4416,7 @@
         <v>8</v>
       </c>
       <c r="B362" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.3">
@@ -4426,7 +4429,7 @@
         <v>0</v>
       </c>
       <c r="B364" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.3">
@@ -4442,7 +4445,7 @@
         <v>2</v>
       </c>
       <c r="B366" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.3">
@@ -4450,7 +4453,7 @@
         <v>3</v>
       </c>
       <c r="B367" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.3">
@@ -4458,7 +4461,7 @@
         <v>4</v>
       </c>
       <c r="B368" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="369" spans="1:6" x14ac:dyDescent="0.3">
@@ -4466,7 +4469,7 @@
         <v>5</v>
       </c>
       <c r="B369" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="370" spans="1:6" x14ac:dyDescent="0.3">
@@ -4474,7 +4477,7 @@
         <v>6</v>
       </c>
       <c r="B370" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="371" spans="1:6" x14ac:dyDescent="0.3">
@@ -4482,7 +4485,7 @@
         <v>7</v>
       </c>
       <c r="B371" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="372" spans="1:6" x14ac:dyDescent="0.3">
@@ -4490,7 +4493,7 @@
         <v>8</v>
       </c>
       <c r="B372" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="373" spans="1:6" x14ac:dyDescent="0.3">
@@ -4498,7 +4501,7 @@
         <v>9</v>
       </c>
       <c r="B373" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="374" spans="1:6" x14ac:dyDescent="0.3">
@@ -4506,7 +4509,7 @@
         <v>10</v>
       </c>
       <c r="B374" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="375" spans="1:6" x14ac:dyDescent="0.3">
@@ -4514,7 +4517,7 @@
         <v>11</v>
       </c>
       <c r="B375" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="376" spans="1:6" x14ac:dyDescent="0.3">
@@ -4522,7 +4525,7 @@
         <v>12</v>
       </c>
       <c r="B376" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="377" spans="1:6" x14ac:dyDescent="0.3">
@@ -4530,7 +4533,7 @@
         <v>13</v>
       </c>
       <c r="B377" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="378" spans="1:6" x14ac:dyDescent="0.3">
@@ -4538,10 +4541,10 @@
         <v>14</v>
       </c>
       <c r="B378" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="D378" s="1" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="E378" s="1"/>
       <c r="F378" s="1"/>
@@ -4551,7 +4554,7 @@
         <v>15</v>
       </c>
       <c r="B379" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="380" spans="1:6" x14ac:dyDescent="0.3">
@@ -4559,7 +4562,7 @@
         <v>16</v>
       </c>
       <c r="B380" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="381" spans="1:6" x14ac:dyDescent="0.3">
@@ -4567,7 +4570,7 @@
         <v>17</v>
       </c>
       <c r="B381" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="382" spans="1:6" x14ac:dyDescent="0.3">
@@ -4575,7 +4578,7 @@
         <v>18</v>
       </c>
       <c r="B382" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="383" spans="1:6" x14ac:dyDescent="0.3">
@@ -4583,7 +4586,7 @@
         <v>19</v>
       </c>
       <c r="B383" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
     <row r="384" spans="1:6" x14ac:dyDescent="0.3">
@@ -4591,7 +4594,7 @@
         <v>20</v>
       </c>
       <c r="B384" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.3">
@@ -4599,7 +4602,7 @@
         <v>21</v>
       </c>
       <c r="B385" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.3">
@@ -4607,7 +4610,7 @@
         <v>22</v>
       </c>
       <c r="B386" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.3">
@@ -4615,7 +4618,7 @@
         <v>23</v>
       </c>
       <c r="B387" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.3">
@@ -4623,7 +4626,7 @@
         <v>24</v>
       </c>
       <c r="B388" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.3">
@@ -4636,7 +4639,7 @@
         <v>1</v>
       </c>
       <c r="B390" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.3">
@@ -4644,7 +4647,7 @@
         <v>2</v>
       </c>
       <c r="B391" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.3">
@@ -4652,12 +4655,12 @@
         <v>3</v>
       </c>
       <c r="B392" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A393" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.3">
@@ -4665,7 +4668,7 @@
         <v>1</v>
       </c>
       <c r="B394" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.3">
@@ -4673,7 +4676,7 @@
         <v>2</v>
       </c>
       <c r="B395" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.3">
@@ -4681,7 +4684,7 @@
         <v>3</v>
       </c>
       <c r="B396" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.3">
@@ -4689,7 +4692,7 @@
         <v>4</v>
       </c>
       <c r="B397" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.3">
@@ -4697,7 +4700,7 @@
         <v>5</v>
       </c>
       <c r="B398" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.3">
@@ -4705,7 +4708,7 @@
         <v>6</v>
       </c>
       <c r="B399" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.3">
@@ -4713,7 +4716,7 @@
         <v>7</v>
       </c>
       <c r="B400" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.3">
@@ -4721,7 +4724,7 @@
         <v>8</v>
       </c>
       <c r="B401" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.3">
@@ -4729,7 +4732,7 @@
         <v>9</v>
       </c>
       <c r="B402" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.3">
@@ -4737,7 +4740,7 @@
         <v>10</v>
       </c>
       <c r="B403" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.3">
@@ -4750,7 +4753,7 @@
         <v>0</v>
       </c>
       <c r="B405" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.3">
@@ -4758,7 +4761,7 @@
         <v>1</v>
       </c>
       <c r="B406" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.3">
@@ -4771,7 +4774,7 @@
         <v>0</v>
       </c>
       <c r="B408" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="409" spans="1:2" x14ac:dyDescent="0.3">
@@ -4779,7 +4782,7 @@
         <v>1</v>
       </c>
       <c r="B409" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.3">
@@ -4792,7 +4795,7 @@
         <v>0</v>
       </c>
       <c r="B411" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.3">
@@ -4800,7 +4803,7 @@
         <v>1</v>
       </c>
       <c r="B412" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>

</xml_diff>